<commit_message>
Reorganising the test decks by format since year decks are removed, as well as adding dates to the formats for chronological sorting. Also, updated the playtest results template to fix Tengu Plant's date.
</commit_message>
<xml_diff>
--- a/Templates/Custom Archetype Template/Playtest Results.xlsx
+++ b/Templates/Custom Archetype Template/Playtest Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Templates\Custom Archetype Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A03656A-7941-41EB-BD60-1814A62307C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B75DB5-6BDB-427A-8B33-DB253A19F412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{AD9CF55C-5A2C-43F9-8449-28DA4DBE7F5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Environment Changes" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="90">
   <si>
     <t>Deck</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Casual</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Tengu Plant's date</t>
   </si>
 </sst>
 </file>
@@ -697,19 +703,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BB1FBB-F5E1-4E55-9B32-F360CDEA6ABD}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.44140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -729,48 +735,56 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
-        <v>45620</v>
+        <v>45726</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>53</v>
       </c>
       <c r="F2" s="11">
         <f>MAX(A:A)</f>
+        <v>45726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>45620</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
       <c r="E3" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="11">
         <f>MAX(INDEX(A:A, MATCH(E3, B:B, 1), 0))</f>
-        <v>45620</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="C7" s="11"/>
     </row>
@@ -787,16 +801,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -804,7 +818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>38565</v>
       </c>
@@ -812,7 +826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>39448</v>
       </c>
@@ -820,7 +834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>39630</v>
       </c>
@@ -828,7 +842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>40269</v>
       </c>
@@ -836,15 +850,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <v>40817</v>
+        <v>40787</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>41821</v>
       </c>
@@ -864,20 +878,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC8C623-D4B8-4C22-A988-D9BD9517564D}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
@@ -897,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>38565</v>
       </c>
@@ -914,7 +928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>38565</v>
       </c>
@@ -931,7 +945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>38565</v>
       </c>
@@ -948,7 +962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>38565</v>
       </c>
@@ -965,7 +979,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>38565</v>
       </c>
@@ -982,7 +996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>38565</v>
       </c>
@@ -999,7 +1013,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>38565</v>
       </c>
@@ -1016,7 +1030,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>38565</v>
       </c>
@@ -1033,7 +1047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>38565</v>
       </c>
@@ -1050,7 +1064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>38565</v>
       </c>
@@ -1070,7 +1084,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>38565</v>
       </c>
@@ -1087,7 +1101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>38565</v>
       </c>
@@ -1104,7 +1118,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>38565</v>
       </c>
@@ -1121,7 +1135,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>38565</v>
       </c>
@@ -1138,7 +1152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>38565</v>
       </c>
@@ -1155,7 +1169,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>38565</v>
       </c>
@@ -1172,7 +1186,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>38565</v>
       </c>
@@ -1189,7 +1203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>38565</v>
       </c>
@@ -1206,7 +1220,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>38565</v>
       </c>
@@ -1223,7 +1237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>38565</v>
       </c>
@@ -1240,7 +1254,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>38565</v>
       </c>
@@ -1257,7 +1271,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>38565</v>
       </c>
@@ -1277,7 +1291,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>38565</v>
       </c>
@@ -1294,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>38565</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>38565</v>
       </c>
@@ -1328,7 +1342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <f>INDEX(Formats!A:A, MATCH(B27, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -1346,7 +1360,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <f>INDEX(Formats!A:A, MATCH(B28, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -1364,7 +1378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <f>INDEX(Formats!A:A, MATCH(B29, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -1382,7 +1396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <f>INDEX(Formats!A:A, MATCH(B30, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -1400,7 +1414,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <f>INDEX(Formats!A:A, MATCH(B31, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -1418,7 +1432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <f>INDEX(Formats!A:A, MATCH(B32, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1436,7 +1450,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <f>INDEX(Formats!A:A, MATCH(B33, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1454,7 +1468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <f>INDEX(Formats!A:A, MATCH(B34, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1472,7 +1486,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <f>INDEX(Formats!A:A, MATCH(B35, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1490,7 +1504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <f>INDEX(Formats!A:A, MATCH(B36, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1508,7 +1522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <f>INDEX(Formats!A:A, MATCH(B37, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1526,7 +1540,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <f>INDEX(Formats!A:A, MATCH(B38, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1544,7 +1558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <f>INDEX(Formats!A:A, MATCH(B39, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1562,7 +1576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <f>INDEX(Formats!A:A, MATCH(B40, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1580,7 +1594,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <f>INDEX(Formats!A:A, MATCH(B41, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1598,7 +1612,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <f>INDEX(Formats!A:A, MATCH(B42, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1616,7 +1630,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <f>INDEX(Formats!A:A, MATCH(B43, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1634,7 +1648,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <f>INDEX(Formats!A:A, MATCH(B44, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1652,7 +1666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <f>INDEX(Formats!A:A, MATCH(B45, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1670,7 +1684,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <f>INDEX(Formats!A:A, MATCH(B46, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1688,7 +1702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <f>INDEX(Formats!A:A, MATCH(B47, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1706,7 +1720,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <f>INDEX(Formats!A:A, MATCH(B48, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1724,7 +1738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <f>INDEX(Formats!A:A, MATCH(B49, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1742,7 +1756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <f>INDEX(Formats!A:A, MATCH(B50, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -1776,15 +1790,15 @@
       <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1810,50 +1824,50 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
     </row>
   </sheetData>
@@ -1873,24 +1887,24 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="8" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1931,7 +1945,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>38565</v>
       </c>
@@ -1980,7 +1994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>38565</v>
       </c>
@@ -2029,7 +2043,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>38565</v>
       </c>
@@ -2078,7 +2092,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>38565</v>
       </c>
@@ -2127,7 +2141,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>38565</v>
       </c>
@@ -2176,7 +2190,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>38565</v>
       </c>
@@ -2225,7 +2239,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>38565</v>
       </c>
@@ -2274,7 +2288,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>38565</v>
       </c>
@@ -2323,7 +2337,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>38565</v>
       </c>
@@ -2372,7 +2386,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>38565</v>
       </c>
@@ -2421,7 +2435,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>38565</v>
       </c>
@@ -2470,7 +2484,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>38565</v>
       </c>
@@ -2519,7 +2533,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>38565</v>
       </c>
@@ -2568,7 +2582,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>38565</v>
       </c>
@@ -2617,7 +2631,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>38565</v>
       </c>
@@ -2666,7 +2680,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>38565</v>
       </c>
@@ -2715,7 +2729,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>38565</v>
       </c>
@@ -2764,7 +2778,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>38565</v>
       </c>
@@ -2813,7 +2827,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>38565</v>
       </c>
@@ -2862,7 +2876,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>38565</v>
       </c>
@@ -2911,7 +2925,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>38565</v>
       </c>
@@ -2960,7 +2974,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>38565</v>
       </c>
@@ -3009,7 +3023,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>38565</v>
       </c>
@@ -3058,7 +3072,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <f>INDEX(Formats!A:A, MATCH(B25, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -3108,7 +3122,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <f>INDEX(Formats!A:A, MATCH(B26, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -3158,7 +3172,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <f>INDEX(Formats!A:A, MATCH(B27, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -3208,7 +3222,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <f>INDEX(Formats!A:A, MATCH(B28, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -3258,7 +3272,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <f>INDEX(Formats!A:A, MATCH(B29, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -3308,7 +3322,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <f>INDEX(Formats!A:A, MATCH(B30, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3355,7 +3369,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <f>INDEX(Formats!A:A, MATCH(B31, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3405,7 +3419,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <f>INDEX(Formats!A:A, MATCH(B32, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3455,7 +3469,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <f>INDEX(Formats!A:A, MATCH(B33, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3505,7 +3519,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <f>INDEX(Formats!A:A, MATCH(B34, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3555,7 +3569,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <f>INDEX(Formats!A:A, MATCH(B35, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3605,7 +3619,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <f>INDEX(Formats!A:A, MATCH(B36, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3655,7 +3669,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <f>INDEX(Formats!A:A, MATCH(B37, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3705,7 +3719,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <f>INDEX(Formats!A:A, MATCH(B38, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3755,7 +3769,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <f>INDEX(Formats!A:A, MATCH(B39, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3805,7 +3819,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <f>INDEX(Formats!A:A, MATCH(B40, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3855,7 +3869,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <f>INDEX(Formats!A:A, MATCH(B41, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3905,7 +3919,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <f>INDEX(Formats!A:A, MATCH(B42, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -3955,7 +3969,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <f>INDEX(Formats!A:A, MATCH(B43, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -4005,7 +4019,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <f>INDEX(Formats!A:A, MATCH(B44, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -4055,7 +4069,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <f>INDEX(Formats!A:A, MATCH(B45, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -4105,7 +4119,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <f>INDEX(Formats!A:A, MATCH(B46, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -4155,7 +4169,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <f>INDEX(Formats!A:A, MATCH(B47, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -4205,7 +4219,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <f>INDEX(Formats!A:A, MATCH(B48, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -4270,26 +4284,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B7D2B9-9D46-4B9E-9494-05F1699F9F2F}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -4324,7 +4338,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <f>INDEX(Formats!A:A, MATCH(B2, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -4368,7 +4382,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <f>INDEX(Formats!A:A, MATCH(B3, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -4412,7 +4426,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <f>INDEX(Formats!A:A, MATCH(B4, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -4456,7 +4470,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <f>INDEX(Formats!A:A, MATCH(B5, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -4480,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="e">
-        <f>D8/SUM(D8+E8)</f>
+        <f t="shared" ref="G5:G19" si="2">D8/SUM(D8+E8)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H5">
@@ -4500,7 +4514,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <f>INDEX(Formats!A:A, MATCH(B6, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -4524,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="e">
-        <f>D9/SUM(D9+E9)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H6">
@@ -4544,7 +4558,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f>INDEX(Formats!A:A, MATCH(B7, Formats!B:B, 0), 0)</f>
         <v>38565</v>
@@ -4568,7 +4582,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="e">
-        <f>D10/SUM(D10+E10)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H7">
@@ -4588,7 +4602,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <f>INDEX(Formats!A:A, MATCH(B8, Formats!B:B, 0), 0)</f>
         <v>39448</v>
@@ -4612,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="e">
-        <f>D11/SUM(D11+E11)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H8">
@@ -4632,7 +4646,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <f>INDEX(Formats!A:A, MATCH(B9, Formats!B:B, 0), 0)</f>
         <v>39448</v>
@@ -4656,7 +4670,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="e">
-        <f>D12/SUM(D12+E12)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H9">
@@ -4676,7 +4690,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <f>INDEX(Formats!A:A, MATCH(B10, Formats!B:B, 0), 0)</f>
         <v>39448</v>
@@ -4700,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="e">
-        <f>D13/SUM(D13+E13)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H10">
@@ -4720,7 +4734,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <f>INDEX(Formats!A:A, MATCH(B11, Formats!B:B, 0), 0)</f>
         <v>39630</v>
@@ -4744,7 +4758,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="e">
-        <f>D14/SUM(D14+E14)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H11">
@@ -4764,7 +4778,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <f>INDEX(Formats!A:A, MATCH(B12, Formats!B:B, 0), 0)</f>
         <v>39630</v>
@@ -4788,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="e">
-        <f>D15/SUM(D15+E15)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H12">
@@ -4808,7 +4822,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <f>INDEX(Formats!A:A, MATCH(B13, Formats!B:B, 0), 0)</f>
         <v>39630</v>
@@ -4832,7 +4846,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="e">
-        <f>D16/SUM(D16+E16)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H13">
@@ -4852,7 +4866,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <f>INDEX(Formats!A:A, MATCH(B14, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -4876,7 +4890,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="e">
-        <f>D17/SUM(D17+E17)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H14">
@@ -4896,7 +4910,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <f>INDEX(Formats!A:A, MATCH(B15, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -4920,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="e">
-        <f>D18/SUM(D18+E18)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H15">
@@ -4940,7 +4954,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <f>INDEX(Formats!A:A, MATCH(B16, Formats!B:B, 0), 0)</f>
         <v>40269</v>
@@ -4964,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="e">
-        <f>D19/SUM(D19+E19)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H16">
@@ -4984,10 +4998,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f>INDEX(Formats!A:A, MATCH(B17, Formats!B:B, 0), 0)</f>
-        <v>40817</v>
+        <v>40787</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
@@ -5008,7 +5022,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="e">
-        <f>D20/SUM(D20+E20)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H17">
@@ -5028,10 +5042,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f>INDEX(Formats!A:A, MATCH(B18, Formats!B:B, 0), 0)</f>
-        <v>40817</v>
+        <v>40787</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -5052,7 +5066,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="e">
-        <f>D21/SUM(D21+E21)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H18">
@@ -5072,10 +5086,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <f>INDEX(Formats!A:A, MATCH(B19, Formats!B:B, 0), 0)</f>
-        <v>40817</v>
+        <v>40787</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
@@ -5096,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="e">
-        <f>D22/SUM(D22+E22)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H19">
@@ -5116,7 +5130,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <f>INDEX(Formats!A:A, MATCH(B20, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -5140,7 +5154,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="e">
-        <f t="shared" ref="G20:G22" si="2">D23/SUM(D23+E23)</f>
+        <f t="shared" ref="G20:G22" si="3">D23/SUM(D23+E23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H20">
@@ -5156,11 +5170,11 @@
         <v>0</v>
       </c>
       <c r="K20" t="e">
-        <f t="shared" ref="K20:K22" si="3">H20/SUM(H20+I20)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" ref="K20:K22" si="4">H20/SUM(H20+I20)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f>INDEX(Formats!A:A, MATCH(B21, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -5184,7 +5198,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H21">
@@ -5200,11 +5214,11 @@
         <v>0</v>
       </c>
       <c r="K21" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <f>INDEX(Formats!A:A, MATCH(B22, Formats!B:B, 0), 0)</f>
         <v>41821</v>
@@ -5228,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H22">
@@ -5244,7 +5258,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>